<commit_message>
Packet extractor tool changes
</commit_message>
<xml_diff>
--- a/packet-extractor/resource/template.xlsx
+++ b/packet-extractor/resource/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Unmatched IdRepo and Packet Info List</t>
   </si>
@@ -22,13 +22,10 @@
     <t>RID</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Demographic Status</t>
   </si>
   <si>
-    <t>Packet Info</t>
-  </si>
-  <si>
-    <t>IdRepo Info</t>
+    <t>Biographic Status</t>
   </si>
 </sst>
 </file>
@@ -36,10 +33,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -58,54 +55,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -119,43 +131,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -172,31 +147,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,13 +208,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,25 +316,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,49 +382,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,92 +392,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -408,6 +405,28 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -416,6 +435,45 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -437,26 +495,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,15 +521,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -511,9 +543,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -522,7 +556,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -534,140 +571,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -677,7 +711,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -999,45 +1039,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="2" width="36.5555555555556" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.7777777777778" style="1" customWidth="1"/>
-    <col min="4" max="4" width="36.4444444444444" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88888888888889" style="1"/>
+    <col min="4" max="16384" width="8.88888888888889" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>